<commit_message>
migrated to .net 6.0 improved errors Added Games tab to excel now posts excel screenshots to discord
</commit_message>
<xml_diff>
--- a/BlockTanksStats/Templates/ClanDashboardTemplate.xlsx
+++ b/BlockTanksStats/Templates/ClanDashboardTemplate.xlsx
@@ -8,21 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peterB\repositories\hobby projecten\BlockTanksStats\BlockTanksStats\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15944424-7839-4983-886E-127A2FB2D60C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839C5CE1-77EA-4F68-A6D3-F2BA047E61AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XP Per Day" sheetId="1" r:id="rId1"/>
     <sheet name="KDR Per Day" sheetId="2" r:id="rId2"/>
+    <sheet name="Games Per Day" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="DatesGAmes">'Games Per Day'!$E$1</definedName>
     <definedName name="DatesKDR">'KDR Per Day'!$D$1</definedName>
-    <definedName name="DatesXP">'XP Per Day'!$E$1</definedName>
+    <definedName name="DatesXP">'XP Per Day'!$E$3</definedName>
+    <definedName name="PlayersGames">'Games Per Day'!$A$2:$E$3</definedName>
+    <definedName name="PlayersGames_Games">'Games Per Day'!$E$2</definedName>
     <definedName name="PlayersKDR">'KDR Per Day'!$A$2:$D$3</definedName>
     <definedName name="PlayersKDR_KDR">'KDR Per Day'!$D$2</definedName>
-    <definedName name="PlayersXP">'XP Per Day'!$A$2:$E$3</definedName>
-    <definedName name="PlayersXP_XP">'XP Per Day'!$E$2</definedName>
+    <definedName name="PlayersXP">'XP Per Day'!$A$4:$E$5</definedName>
+    <definedName name="PlayersXP_XP">'XP Per Day'!$E$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>{{item.CurrentTotalXp}}</t>
   </si>
@@ -76,13 +80,28 @@
   </si>
   <si>
     <t>&amp;=IF(SUM(PlayersXP_XP) = 0, 0, AVERAGE(PlayersXP_XP))&lt;&lt;OnlyValues&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Highlight upperbound:</t>
+  </si>
+  <si>
+    <t>Total Games</t>
+  </si>
+  <si>
+    <t>Average Games</t>
+  </si>
+  <si>
+    <t>&amp;=IF(SUM(PlayersGames_Games) = 0, 0, AVERAGE(PlayersGames_Games))&lt;&lt;OnlyValues&gt;&gt;</t>
+  </si>
+  <si>
+    <t>{{item.CurrentTotalGames}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,16 +117,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -115,11 +146,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -136,11 +183,30 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -418,14 +484,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="2" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="3" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="3" customWidth="1"/>
@@ -454,41 +520,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="13">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -503,6 +575,15 @@
     </row>
   </sheetData>
   <dataConsolidate/>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="between">
+      <formula>0</formula>
+      <formula>$C$1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -512,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FECE3695-A7AD-4B4C-B9BA-D67F2C2083B1}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -556,4 +637,64 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828C5977-CB44-48E3-8F8C-CDA55B340702}">
+  <dimension ref="B1:E3"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>